<commit_message>
Deploying to gh-pages from  @ e3d5e1e744a47bdc56a014b3bdfe405b221a4fb8 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/4.1.1.1a.xlsx
+++ b/en/downloads/data-excel/4.1.1.1a.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="69">
   <si>
     <t xml:space="preserve">4.1.1.1а Жалпы билим берүү уюмдарынын сабактарына барбай калган балдардын жана 7-17 жаштагы (1-11-класстардагы) өспүрүмдөрдүн  себептер жана жынысы боюнча саны </t>
   </si>
@@ -395,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -538,6 +538,25 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -843,9 +862,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -856,7 +877,7 @@
     <col min="6" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="51" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +903,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -908,7 +929,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -927,8 +948,9 @@
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S3" s="54"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -983,8 +1005,11 @@
       <c r="R4" s="15">
         <v>2019</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="48">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -1009,8 +1034,9 @@
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
       <c r="R5" s="19"/>
-    </row>
-    <row r="6" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S5" s="49"/>
+    </row>
+    <row r="6" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
@@ -1065,8 +1091,11 @@
       <c r="R6" s="24">
         <v>1662</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="50">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
@@ -1091,8 +1120,9 @@
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
       <c r="R7" s="31"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="51"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>18</v>
       </c>
@@ -1147,8 +1177,11 @@
       <c r="R8" s="31">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="51">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>21</v>
       </c>
@@ -1203,8 +1236,11 @@
       <c r="R9" s="31">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S9" s="51">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>24</v>
       </c>
@@ -1256,11 +1292,14 @@
       <c r="Q10" s="31">
         <v>4</v>
       </c>
-      <c r="R10" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S10" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>28</v>
       </c>
@@ -1315,8 +1354,11 @@
       <c r="R11" s="31">
         <v>374</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="51">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>31</v>
       </c>
@@ -1371,8 +1413,11 @@
       <c r="R12" s="31">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="51">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>34</v>
       </c>
@@ -1427,8 +1472,11 @@
       <c r="R13" s="31">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>37</v>
       </c>
@@ -1483,8 +1531,11 @@
       <c r="R14" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S14" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>40</v>
       </c>
@@ -1539,8 +1590,11 @@
       <c r="R15" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>43</v>
       </c>
@@ -1595,8 +1649,11 @@
       <c r="R16" s="31">
         <v>121</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S16" s="51">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>46</v>
       </c>
@@ -1648,11 +1705,14 @@
       <c r="Q17" s="31">
         <v>3</v>
       </c>
-      <c r="R17" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="R17" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S17" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>48</v>
       </c>
@@ -1707,8 +1767,11 @@
       <c r="R18" s="31">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>51</v>
       </c>
@@ -1763,8 +1826,11 @@
       <c r="R19" s="31">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>54</v>
       </c>
@@ -1819,8 +1885,11 @@
       <c r="R20" s="31">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>57</v>
       </c>
@@ -1875,8 +1944,11 @@
       <c r="R21" s="31">
         <v>906</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="51">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>60</v>
       </c>
@@ -1931,8 +2003,11 @@
       <c r="R22" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>63</v>
       </c>
@@ -1957,8 +2032,9 @@
       <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
       <c r="R23" s="19"/>
-    </row>
-    <row r="24" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S23" s="49"/>
+    </row>
+    <row r="24" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>12</v>
       </c>
@@ -2013,8 +2089,11 @@
       <c r="R24" s="24">
         <v>1172</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="50">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>15</v>
       </c>
@@ -2039,8 +2118,9 @@
       <c r="P25" s="31"/>
       <c r="Q25" s="31"/>
       <c r="R25" s="31"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="51"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>18</v>
       </c>
@@ -2095,8 +2175,11 @@
       <c r="R26" s="31">
         <v>110</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="51">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>21</v>
       </c>
@@ -2151,8 +2234,11 @@
       <c r="R27" s="31">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S27" s="51">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
         <v>24</v>
       </c>
@@ -2191,8 +2277,11 @@
       <c r="R28" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>28</v>
       </c>
@@ -2247,8 +2336,11 @@
       <c r="R29" s="31">
         <v>260</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="51">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>31</v>
       </c>
@@ -2303,8 +2395,11 @@
       <c r="R30" s="31">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="51">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>34</v>
       </c>
@@ -2359,8 +2454,11 @@
       <c r="R31" s="31">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="51">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>37</v>
       </c>
@@ -2415,8 +2513,11 @@
       <c r="R32" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S32" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>40</v>
       </c>
@@ -2455,8 +2556,11 @@
       <c r="R33" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>43</v>
       </c>
@@ -2511,8 +2615,11 @@
       <c r="R34" s="31">
         <v>91</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S34" s="51">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>46</v>
       </c>
@@ -2551,8 +2658,11 @@
       <c r="R35" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="S35" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>48</v>
       </c>
@@ -2591,8 +2701,11 @@
       <c r="R36" s="31">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
         <v>51</v>
       </c>
@@ -2631,8 +2744,11 @@
       <c r="R37" s="31">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>54</v>
       </c>
@@ -2687,8 +2803,11 @@
       <c r="R38" s="31">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38" s="51">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>57</v>
       </c>
@@ -2743,8 +2862,11 @@
       <c r="R39" s="31">
         <v>615</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S39" s="51">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>60</v>
       </c>
@@ -2799,8 +2921,11 @@
       <c r="R40" s="45" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40" s="53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 0d0ffeaff9e0087f25ede5ade66aaa8603c52931 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/4.1.1.1a.xlsx
+++ b/en/downloads/data-excel/4.1.1.1a.xlsx
@@ -14,13 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="69">
   <si>
     <t xml:space="preserve">4.1.1.1а Жалпы билим берүү уюмдарынын сабактарына барбай калган балдардын жана 7-17 жаштагы (1-11-класстардагы) өспүрүмдөрдүн  себептер жана жынысы боюнча саны </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.1.1.1а Численность детей и подростков 7-17 лет (1-11классов), не приступивших  к занятиям 
-в общеобразовательные организации по причинам,  по полу </t>
   </si>
   <si>
     <t>4.1.1.1а Number of children (1-11 classes)  not started studies at school by cause,  sex and territory</t>
@@ -223,6 +219,9 @@
   </si>
   <si>
     <t>Note : Data on the floor began to be developed from 2005 .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1.1.1а Численность детей и подростков 7-17 лет (1-11классов), не приступивших  к занятиям в общеобразовательные организации по причинам,  по полу </t>
   </si>
 </sst>
 </file>
@@ -865,30 +864,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.7109375" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" customWidth="1"/>
-    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="9" width="9.7109375" customWidth="1"/>
+    <col min="1" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="8" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -906,15 +902,15 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -932,12 +928,12 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -954,21 +950,22 @@
       <c r="S3" s="54"/>
       <c r="T3" s="54"/>
       <c r="U3" s="54"/>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V3" s="54"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="14">
+      <c r="D4" s="15">
         <v>2005</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="15">
         <v>2006</v>
       </c>
       <c r="F4" s="15">
@@ -1019,16 +1016,19 @@
       <c r="U4" s="48">
         <v>2022</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" s="48">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -1048,16 +1048,17 @@
       <c r="S5" s="49"/>
       <c r="T5" s="49"/>
       <c r="U5" s="49"/>
-    </row>
-    <row r="6" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+      <c r="V5" s="49"/>
+    </row>
+    <row r="6" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="C6" s="22" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>14</v>
       </c>
       <c r="D6" s="23">
         <v>2331</v>
@@ -1113,16 +1114,19 @@
       <c r="U6" s="55">
         <v>1456</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" s="55">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="C7" s="29" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>17</v>
       </c>
       <c r="D7" s="30"/>
       <c r="E7" s="18"/>
@@ -1142,16 +1146,17 @@
       <c r="S7" s="51"/>
       <c r="T7" s="52"/>
       <c r="U7" s="52"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7" s="52"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="C8" s="29" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>20</v>
       </c>
       <c r="D8" s="30">
         <v>295</v>
@@ -1207,16 +1212,19 @@
       <c r="U8" s="52">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" s="52">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="C9" s="29" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>23</v>
       </c>
       <c r="D9" s="30">
         <v>86</v>
@@ -1272,40 +1280,43 @@
       <c r="U9" s="52">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+      <c r="V9" s="52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="C10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10" s="31">
         <v>3</v>
@@ -1320,33 +1331,36 @@
         <v>3</v>
       </c>
       <c r="P10" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q10" s="31">
         <v>4</v>
       </c>
       <c r="R10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S10" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T10" s="52">
         <v>1</v>
       </c>
       <c r="U10" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="B11" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="C11" s="29" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>30</v>
       </c>
       <c r="D11" s="30">
         <v>208</v>
@@ -1402,16 +1416,19 @@
       <c r="U11" s="52">
         <v>217</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" s="52">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="C12" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>33</v>
       </c>
       <c r="D12" s="30">
         <v>222</v>
@@ -1467,16 +1484,19 @@
       <c r="U12" s="52">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V12" s="52">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>36</v>
       </c>
       <c r="D13" s="30">
         <v>87</v>
@@ -1532,16 +1552,19 @@
       <c r="U13" s="52">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13" s="52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>39</v>
       </c>
       <c r="D14" s="30">
         <v>11</v>
@@ -1571,107 +1594,113 @@
         <v>6</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N14" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P14" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q14" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R14" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S14" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T14" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U14" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V14" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="C15" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>42</v>
-      </c>
       <c r="D15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M15" s="18">
         <v>3</v>
       </c>
       <c r="N15" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P15" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R15" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S15" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T15" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U15" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V15" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="C16" s="37" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>45</v>
       </c>
       <c r="D16" s="30">
         <v>102</v>
@@ -1727,40 +1756,43 @@
       <c r="U16" s="52">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+      <c r="V16" s="52">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="35" t="s">
-        <v>47</v>
-      </c>
       <c r="C17" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L17" s="31">
         <v>2</v>
@@ -1769,63 +1801,66 @@
         <v>3</v>
       </c>
       <c r="N17" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O17" s="33">
         <v>2</v>
       </c>
       <c r="P17" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q17" s="31">
         <v>3</v>
       </c>
       <c r="R17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S17" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T17" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U17" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V17" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="C18" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="36" t="s">
-        <v>50</v>
-      </c>
       <c r="D18" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L18" s="31">
         <v>19</v>
@@ -1857,40 +1892,43 @@
       <c r="U18" s="52">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="C19" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="38" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L19" s="31">
         <v>2</v>
@@ -1905,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="P19" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q19" s="31">
         <v>20</v>
@@ -1917,21 +1955,24 @@
         <v>6</v>
       </c>
       <c r="T19" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U19" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V19" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="C20" s="37" t="s">
         <v>55</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>56</v>
       </c>
       <c r="D20" s="39">
         <v>310</v>
@@ -1987,16 +2028,19 @@
       <c r="U20" s="52">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V20" s="52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="C21" s="38" t="s">
         <v>58</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>59</v>
       </c>
       <c r="D21" s="18">
         <v>908</v>
@@ -2052,16 +2096,19 @@
       <c r="U21" s="52">
         <v>1021</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V21" s="52">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="C22" s="29" t="s">
         <v>61</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>62</v>
       </c>
       <c r="D22" s="30">
         <v>102</v>
@@ -2088,45 +2135,48 @@
         <v>174</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N22" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O22" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P22" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q22" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R22" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S22" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T22" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U22" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V22" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>65</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -2146,16 +2196,17 @@
       <c r="S23" s="49"/>
       <c r="T23" s="49"/>
       <c r="U23" s="49"/>
-    </row>
-    <row r="24" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+      <c r="V23" s="49"/>
+    </row>
+    <row r="24" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="C24" s="22" t="s">
         <v>13</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>14</v>
       </c>
       <c r="D24" s="23">
         <v>1360</v>
@@ -2211,16 +2262,19 @@
       <c r="U24" s="55">
         <v>1019</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="55">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="C25" s="29" t="s">
         <v>16</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>17</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="18"/>
@@ -2240,16 +2294,17 @@
       <c r="S25" s="51"/>
       <c r="T25" s="52"/>
       <c r="U25" s="52"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="52"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="C26" s="29" t="s">
         <v>19</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>20</v>
       </c>
       <c r="D26" s="30">
         <v>137</v>
@@ -2305,16 +2360,19 @@
       <c r="U26" s="52">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" s="52">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="C27" s="29" t="s">
         <v>22</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>23</v>
       </c>
       <c r="D27" s="30">
         <v>41</v>
@@ -2370,16 +2428,19 @@
       <c r="U27" s="52">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+      <c r="V27" s="52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="C28" s="36" t="s">
         <v>25</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>26</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="18"/>
@@ -2393,7 +2454,7 @@
         <v>5</v>
       </c>
       <c r="M28" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N28" s="18">
         <v>3</v>
@@ -2402,33 +2463,36 @@
         <v>6</v>
       </c>
       <c r="P28" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q28" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R28" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S28" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T28" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U28" s="52">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="C29" s="29" t="s">
         <v>29</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>30</v>
       </c>
       <c r="D29" s="30">
         <v>116</v>
@@ -2484,16 +2548,19 @@
       <c r="U29" s="52">
         <v>179</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="52">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="C30" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>33</v>
       </c>
       <c r="D30" s="30">
         <v>64</v>
@@ -2549,16 +2616,19 @@
       <c r="U30" s="52">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V30" s="52">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="C31" s="29" t="s">
         <v>35</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>36</v>
       </c>
       <c r="D31" s="30">
         <v>31</v>
@@ -2614,16 +2684,19 @@
       <c r="U31" s="52">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V31" s="52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="C32" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>39</v>
       </c>
       <c r="D32" s="30">
         <v>14</v>
@@ -2656,39 +2729,42 @@
         <v>1</v>
       </c>
       <c r="N32" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O32" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P32" s="18">
         <v>1</v>
       </c>
       <c r="Q32" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R32" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S32" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T32" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U32" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V32" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="C33" s="36" t="s">
         <v>41</v>
-      </c>
-      <c r="C33" s="36" t="s">
-        <v>42</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="18"/>
@@ -2705,39 +2781,42 @@
         <v>3</v>
       </c>
       <c r="N33" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O33" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P33" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q33" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R33" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S33" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T33" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U33" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V33" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="C34" s="37" t="s">
         <v>44</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>45</v>
       </c>
       <c r="D34" s="30">
         <v>39</v>
@@ -2793,16 +2872,19 @@
       <c r="U34" s="52">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+      <c r="V34" s="52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="35" t="s">
-        <v>47</v>
-      </c>
       <c r="C35" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="30"/>
       <c r="E35" s="18"/>
@@ -2813,45 +2895,48 @@
       <c r="J35" s="31"/>
       <c r="K35" s="31"/>
       <c r="L35" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N35" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P35" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q35" s="31">
         <v>2</v>
       </c>
       <c r="R35" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S35" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T35" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U35" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V35" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="24" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="C36" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="C36" s="36" t="s">
-        <v>50</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="18"/>
@@ -2871,7 +2956,7 @@
         <v>79</v>
       </c>
       <c r="O36" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P36" s="18">
         <v>1</v>
@@ -2883,24 +2968,27 @@
         <v>8</v>
       </c>
       <c r="S36" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T36" s="52">
         <v>3</v>
       </c>
       <c r="U36" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V36" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="C37" s="38" t="s">
         <v>52</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>53</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="18"/>
@@ -2911,7 +2999,7 @@
       <c r="J37" s="31"/>
       <c r="K37" s="31"/>
       <c r="L37" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M37" s="18">
         <v>4</v>
@@ -2920,7 +3008,7 @@
         <v>2</v>
       </c>
       <c r="O37" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P37" s="18">
         <v>1</v>
@@ -2935,21 +3023,24 @@
         <v>3</v>
       </c>
       <c r="T37" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U37" s="52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V37" s="52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="C38" s="37" t="s">
         <v>55</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>56</v>
       </c>
       <c r="D38" s="39">
         <v>196</v>
@@ -3005,16 +3096,19 @@
       <c r="U38" s="52">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V38" s="52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="C39" s="38" t="s">
         <v>58</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>59</v>
       </c>
       <c r="D39" s="18">
         <v>658</v>
@@ -3070,16 +3164,19 @@
       <c r="U39" s="52">
         <v>699</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V39" s="52">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="C40" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="C40" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="D40" s="44">
         <v>64</v>
@@ -3106,45 +3203,48 @@
         <v>158</v>
       </c>
       <c r="L40" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M40" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N40" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O40" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P40" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q40" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R40" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S40" s="53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T40" s="53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U40" s="53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="V40" s="53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="C41" s="47" t="s">
         <v>67</v>
-      </c>
-      <c r="C41" s="47" t="s">
-        <v>68</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>

</xml_diff>